<commit_message>
Reorganized the markdown file
</commit_message>
<xml_diff>
--- a/data/FlFsFrSummary.xlsx
+++ b/data/FlFsFrSummary.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10812"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jian107/PNNL/GlobalC/data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DACEFEE6-CB05-D44A-BFFA-5EF9624EDA51}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="16440" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="18580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FlFsFrSummary" sheetId="1" r:id="rId1"/>
@@ -18,7 +24,7 @@
     <definedName name="_0raw_2" localSheetId="1">RaGPP!$C$90:$F$107</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">FromSRDB!$A$1:$DE$89</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -31,8 +37,8 @@
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" name="0raw" type="6" refreshedVersion="4" background="1" saveData="1">
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
+  <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" name="0raw" type="6" refreshedVersion="4" background="1" saveData="1">
     <textPr codePage="437" firstRow="2" sourceFile="G:\My Drive\MyResearch\Papers\2.SoilRespiration\FsFfandFw\0Figures\0raw.txt" comma="1">
       <textFields count="2">
         <textField/>
@@ -40,7 +46,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="2" name="0raw1" type="6" refreshedVersion="4" background="1" saveData="1">
+  <connection id="2" xr16:uid="{00000000-0015-0000-FFFF-FFFF01000000}" name="0raw1" type="6" refreshedVersion="4" background="1" saveData="1">
     <textPr codePage="437" firstRow="2" sourceFile="G:\My Drive\MyResearch\Papers\2.SoilRespiration\FsFfandFw\0Figures\0raw.txt" comma="1">
       <textFields count="2">
         <textField/>
@@ -48,7 +54,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="3" name="0raw2" type="6" refreshedVersion="4" background="1" saveData="1">
+  <connection id="3" xr16:uid="{00000000-0015-0000-FFFF-FFFF02000000}" name="0raw2" type="6" refreshedVersion="4" background="1" saveData="1">
     <textPr codePage="437" firstRow="2" sourceFile="G:\My Drive\MyResearch\Papers\2.SoilRespiration\FsFfandFw\0Figures\0raw.txt" comma="1">
       <textFields count="2">
         <textField/>
@@ -1562,7 +1568,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -2172,7 +2178,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1" readingOrder="1"/>
@@ -2202,6 +2208,10 @@
     <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="11" fontId="0" fillId="35" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="19" fillId="34" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1" readingOrder="1"/>
       <protection locked="0"/>
@@ -2230,51 +2240,50 @@
       <alignment vertical="top" wrapText="1" readingOrder="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="35" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20% - 强调文字颜色 1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - 强调文字颜色 2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - 强调文字颜色 3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - 强调文字颜色 4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - 强调文字颜色 5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - 强调文字颜色 6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - 强调文字颜色 1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - 强调文字颜色 2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - 强调文字颜色 3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - 强调文字颜色 4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - 强调文字颜色 5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - 强调文字颜色 6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - 强调文字颜色 2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - 强调文字颜色 3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - 强调文字颜色 4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - 强调文字颜色 5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - 强调文字颜色 6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="好" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="差" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="强调文字颜色 1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="强调文字颜色 2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="强调文字颜色 3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="强调文字颜色 4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="强调文字颜色 5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="强调文字颜色 6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="标题" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="标题 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="标题 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="标题 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="标题 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="检查单元格" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="汇总" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="解释性文本" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="警告文本" xfId="14" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="计算" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="输入" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="输出" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="适中" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="链接单元格" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2290,15 +2299,15 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="0raw_1" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="0raw_2" connectionId="3" xr16:uid="{00000000-0016-0000-0100-000000000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="0raw" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="0raw_1" connectionId="2" xr16:uid="{00000000-0016-0000-0100-000002000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="0raw_2" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="0raw" connectionId="1" xr16:uid="{00000000-0016-0000-0100-000001000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2590,29 +2599,29 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R36"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q30" sqref="Q30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="4" width="11" style="8"/>
-    <col min="7" max="7" width="28.125" customWidth="1"/>
+    <col min="7" max="7" width="28.1640625" customWidth="1"/>
     <col min="10" max="10" width="32" customWidth="1"/>
-    <col min="11" max="11" width="13.625" customWidth="1"/>
+    <col min="11" max="11" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -2668,7 +2677,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="C2" s="8">
         <v>50</v>
       </c>
@@ -2697,7 +2706,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" s="8">
         <v>53</v>
       </c>
@@ -2732,7 +2741,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="C4" s="8">
         <v>55</v>
       </c>
@@ -2761,13 +2770,17 @@
         <v>118</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" s="8">
         <v>28</v>
       </c>
       <c r="B5" s="8">
         <v>26</v>
       </c>
+      <c r="C5" s="13">
+        <f>100-D5</f>
+        <v>54</v>
+      </c>
       <c r="D5" s="8">
         <v>46</v>
       </c>
@@ -2790,13 +2803,17 @@
         <v>118</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" s="8">
         <v>33.5</v>
       </c>
       <c r="B6" s="8">
         <v>39</v>
       </c>
+      <c r="C6" s="13">
+        <f t="shared" ref="C6:C36" si="0">100-D6</f>
+        <v>72.5</v>
+      </c>
       <c r="D6" s="8">
         <v>27.5</v>
       </c>
@@ -2819,13 +2836,17 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" s="8">
         <v>31.6</v>
       </c>
       <c r="B7" s="8">
         <v>39.4</v>
       </c>
+      <c r="C7" s="13">
+        <f t="shared" si="0"/>
+        <v>71</v>
+      </c>
       <c r="D7" s="8">
         <v>29</v>
       </c>
@@ -2851,13 +2872,17 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8" s="8">
         <v>43.17</v>
       </c>
       <c r="B8" s="8">
         <v>34.53</v>
       </c>
+      <c r="C8" s="13">
+        <f t="shared" si="0"/>
+        <v>77.7</v>
+      </c>
       <c r="D8" s="8">
         <v>22.3</v>
       </c>
@@ -2883,7 +2908,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9" s="8">
         <f>M9/P9*100</f>
         <v>41.566265060240966</v>
@@ -2892,6 +2917,10 @@
         <f>N9/P9*100</f>
         <v>12.409638554216867</v>
       </c>
+      <c r="C9" s="13">
+        <f t="shared" si="0"/>
+        <v>53.975903614457835</v>
+      </c>
       <c r="D9" s="8">
         <f>O9/P9*100</f>
         <v>46.024096385542165</v>
@@ -2936,17 +2965,21 @@
         <v>108</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10" s="8">
-        <f t="shared" ref="A10:A14" si="0">M10/P10*100</f>
+        <f t="shared" ref="A10:A14" si="1">M10/P10*100</f>
         <v>48.387096774193552</v>
       </c>
       <c r="B10" s="8">
-        <f t="shared" ref="B10:B14" si="1">N10/P10*100</f>
+        <f t="shared" ref="B10:B14" si="2">N10/P10*100</f>
         <v>3.3794162826420893</v>
       </c>
+      <c r="C10" s="13">
+        <f t="shared" si="0"/>
+        <v>51.766513056835642</v>
+      </c>
       <c r="D10" s="8">
-        <f t="shared" ref="D10:D14" si="2">O10/P10*100</f>
+        <f t="shared" ref="D10:D14" si="3">O10/P10*100</f>
         <v>48.233486943164358</v>
       </c>
       <c r="E10" t="s">
@@ -2959,11 +2992,11 @@
         <v>112</v>
       </c>
       <c r="H10">
-        <f t="shared" ref="H10:H11" si="3">55+53/60</f>
+        <f t="shared" ref="H10:H11" si="4">55+53/60</f>
         <v>55.883333333333333</v>
       </c>
       <c r="I10">
-        <f t="shared" ref="I10:I11" si="4">-98-20/60</f>
+        <f t="shared" ref="I10:I11" si="5">-98-20/60</f>
         <v>-98.333333333333329</v>
       </c>
       <c r="J10" t="s">
@@ -2973,7 +3006,7 @@
         <v>2</v>
       </c>
       <c r="M10">
-        <f t="shared" ref="M10:M14" si="5">P10-N10-O10</f>
+        <f t="shared" ref="M10:M14" si="6">P10-N10-O10</f>
         <v>315</v>
       </c>
       <c r="N10">
@@ -2989,17 +3022,21 @@
         <v>108</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11" s="8">
+        <f t="shared" si="1"/>
+        <v>46.963562753036435</v>
+      </c>
+      <c r="B11" s="8">
+        <f t="shared" si="2"/>
+        <v>10.39136302294197</v>
+      </c>
+      <c r="C11" s="13">
         <f t="shared" si="0"/>
-        <v>46.963562753036435</v>
-      </c>
-      <c r="B11" s="8">
-        <f t="shared" si="1"/>
-        <v>10.39136302294197</v>
+        <v>57.354925775978401</v>
       </c>
       <c r="D11" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>42.645074224021599</v>
       </c>
       <c r="E11" t="s">
@@ -3012,11 +3049,11 @@
         <v>113</v>
       </c>
       <c r="H11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>55.883333333333333</v>
       </c>
       <c r="I11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-98.333333333333329</v>
       </c>
       <c r="J11" t="s">
@@ -3026,7 +3063,7 @@
         <v>2</v>
       </c>
       <c r="M11">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>348</v>
       </c>
       <c r="N11">
@@ -3042,17 +3079,21 @@
         <v>108</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12" s="8">
+        <f t="shared" si="1"/>
+        <v>64.458598726114644</v>
+      </c>
+      <c r="B12" s="8">
+        <f t="shared" si="2"/>
+        <v>11.082802547770701</v>
+      </c>
+      <c r="C12" s="13">
         <f t="shared" si="0"/>
-        <v>64.458598726114644</v>
-      </c>
-      <c r="B12" s="8">
-        <f t="shared" si="1"/>
-        <v>11.082802547770701</v>
+        <v>75.541401273885356</v>
       </c>
       <c r="D12" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>24.458598726114651</v>
       </c>
       <c r="E12" t="s">
@@ -3079,7 +3120,7 @@
         <v>2</v>
       </c>
       <c r="M12">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>506</v>
       </c>
       <c r="N12">
@@ -3095,17 +3136,21 @@
         <v>108</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A13" s="8">
+        <f t="shared" si="1"/>
+        <v>66.168224299065429</v>
+      </c>
+      <c r="B13" s="8">
+        <f t="shared" si="2"/>
+        <v>5.6074766355140184</v>
+      </c>
+      <c r="C13" s="13">
         <f t="shared" si="0"/>
-        <v>66.168224299065429</v>
-      </c>
-      <c r="B13" s="8">
-        <f t="shared" si="1"/>
-        <v>5.6074766355140184</v>
+        <v>71.775700934579447</v>
       </c>
       <c r="D13" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>28.22429906542056</v>
       </c>
       <c r="E13" t="s">
@@ -3118,11 +3163,11 @@
         <v>115</v>
       </c>
       <c r="H13">
-        <f t="shared" ref="H13:H14" si="6">53+53/60</f>
+        <f t="shared" ref="H13:H14" si="7">53+53/60</f>
         <v>53.883333333333333</v>
       </c>
       <c r="I13">
-        <f t="shared" ref="I13:I14" si="7">-104-53/60</f>
+        <f t="shared" ref="I13:I14" si="8">-104-53/60</f>
         <v>-104.88333333333334</v>
       </c>
       <c r="J13" t="s">
@@ -3132,7 +3177,7 @@
         <v>2</v>
       </c>
       <c r="M13">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>354</v>
       </c>
       <c r="N13">
@@ -3148,17 +3193,21 @@
         <v>108</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A14" s="8">
+        <f t="shared" si="1"/>
+        <v>51.872246696035241</v>
+      </c>
+      <c r="B14" s="8">
+        <f t="shared" si="2"/>
+        <v>13.546255506607929</v>
+      </c>
+      <c r="C14" s="13">
         <f t="shared" si="0"/>
-        <v>51.872246696035241</v>
-      </c>
-      <c r="B14" s="8">
-        <f t="shared" si="1"/>
-        <v>13.546255506607929</v>
+        <v>65.418502202643168</v>
       </c>
       <c r="D14" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>34.581497797356832</v>
       </c>
       <c r="E14" t="s">
@@ -3171,11 +3220,11 @@
         <v>116</v>
       </c>
       <c r="H14">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>53.883333333333333</v>
       </c>
       <c r="I14">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>-104.88333333333334</v>
       </c>
       <c r="J14" t="s">
@@ -3185,7 +3234,7 @@
         <v>2</v>
       </c>
       <c r="M14">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>471</v>
       </c>
       <c r="N14">
@@ -3201,13 +3250,17 @@
         <v>108</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A15" s="8">
         <v>32.92</v>
       </c>
       <c r="B15" s="8">
         <v>13.6</v>
       </c>
+      <c r="C15" s="13">
+        <f t="shared" si="0"/>
+        <v>46.52</v>
+      </c>
       <c r="D15" s="8">
         <v>53.48</v>
       </c>
@@ -3233,7 +3286,11 @@
         <v>1470</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="C16" s="13">
+        <f t="shared" si="0"/>
+        <v>75.08</v>
+      </c>
       <c r="D16" s="8">
         <v>24.92</v>
       </c>
@@ -3259,7 +3316,11 @@
         <v>6029</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="C17" s="13">
+        <f t="shared" si="0"/>
+        <v>53.3</v>
+      </c>
       <c r="D17" s="8">
         <v>46.7</v>
       </c>
@@ -3285,13 +3346,17 @@
         <v>1602</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" s="8">
         <v>23.3</v>
       </c>
       <c r="B18" s="8">
         <v>6.7</v>
       </c>
+      <c r="C18" s="13">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
       <c r="D18" s="8">
         <v>70</v>
       </c>
@@ -3317,13 +3382,17 @@
         <v>2241</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" s="8">
         <v>24.4</v>
       </c>
       <c r="B19" s="8">
         <v>18.28</v>
       </c>
+      <c r="C19" s="13">
+        <f t="shared" si="0"/>
+        <v>42.68</v>
+      </c>
       <c r="D19" s="8">
         <v>57.32</v>
       </c>
@@ -3349,13 +3418,17 @@
         <v>2532</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" s="8">
         <v>31.27</v>
       </c>
       <c r="B20" s="8">
         <v>26.01</v>
       </c>
+      <c r="C20" s="13">
+        <f t="shared" si="0"/>
+        <v>57.28</v>
+      </c>
       <c r="D20" s="8">
         <v>42.72</v>
       </c>
@@ -3381,7 +3454,11 @@
         <v>2904</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="C21" s="13">
+        <f t="shared" si="0"/>
+        <v>70.989999999999995</v>
+      </c>
       <c r="D21" s="8">
         <v>29.01</v>
       </c>
@@ -3407,7 +3484,11 @@
         <v>3301</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="C22" s="13">
+        <f t="shared" si="0"/>
+        <v>65.22</v>
+      </c>
       <c r="D22" s="8">
         <v>34.78</v>
       </c>
@@ -3433,7 +3514,11 @@
         <v>3503</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="C23" s="13">
+        <f t="shared" si="0"/>
+        <v>50.96</v>
+      </c>
       <c r="D23" s="8">
         <v>49.04</v>
       </c>
@@ -3459,7 +3544,11 @@
         <v>3705</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="C24" s="13">
+        <f t="shared" si="0"/>
+        <v>63.57</v>
+      </c>
       <c r="D24" s="8">
         <v>36.43</v>
       </c>
@@ -3485,13 +3574,17 @@
         <v>3885</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" s="8">
         <v>46.22</v>
       </c>
       <c r="B25" s="8">
         <v>17.07</v>
       </c>
+      <c r="C25" s="13">
+        <f t="shared" si="0"/>
+        <v>63.29</v>
+      </c>
       <c r="D25" s="8">
         <v>36.71</v>
       </c>
@@ -3517,13 +3610,17 @@
         <v>4166</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" s="8">
         <v>38.1</v>
       </c>
       <c r="B26" s="8">
         <v>26.33</v>
       </c>
+      <c r="C26" s="13">
+        <f t="shared" si="0"/>
+        <v>64.430000000000007</v>
+      </c>
       <c r="D26" s="8">
         <v>35.57</v>
       </c>
@@ -3549,13 +3646,17 @@
         <v>4920</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" s="8">
         <v>41.49</v>
       </c>
       <c r="B27" s="8">
         <v>12.04</v>
       </c>
+      <c r="C27" s="13">
+        <f t="shared" si="0"/>
+        <v>53.53</v>
+      </c>
       <c r="D27" s="8">
         <v>46.47</v>
       </c>
@@ -3581,13 +3682,17 @@
         <v>4938</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" s="8">
         <v>50.51</v>
       </c>
       <c r="B28" s="8">
         <v>21.21</v>
       </c>
+      <c r="C28" s="13">
+        <f t="shared" si="0"/>
+        <v>71.72</v>
+      </c>
       <c r="D28" s="8">
         <v>28.28</v>
       </c>
@@ -3613,13 +3718,17 @@
         <v>4979</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" s="8">
         <v>24.86</v>
       </c>
       <c r="B29" s="8">
         <v>25.15</v>
       </c>
+      <c r="C29" s="13">
+        <f t="shared" si="0"/>
+        <v>50.01</v>
+      </c>
       <c r="D29" s="8">
         <v>49.99</v>
       </c>
@@ -3645,7 +3754,11 @@
         <v>5227</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="C30" s="13">
+        <f t="shared" si="0"/>
+        <v>63.79</v>
+      </c>
       <c r="D30" s="8">
         <v>36.21</v>
       </c>
@@ -3671,13 +3784,17 @@
         <v>5262</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31" s="8">
         <v>50</v>
       </c>
       <c r="B31" s="8">
         <v>15.45</v>
       </c>
+      <c r="C31" s="13">
+        <f t="shared" si="0"/>
+        <v>65.45</v>
+      </c>
       <c r="D31" s="8">
         <v>34.549999999999997</v>
       </c>
@@ -3703,13 +3820,17 @@
         <v>5392</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32" s="8">
         <v>22.96</v>
       </c>
       <c r="B32" s="8">
         <v>34.31</v>
       </c>
+      <c r="C32" s="13">
+        <f t="shared" si="0"/>
+        <v>57.27</v>
+      </c>
       <c r="D32" s="8">
         <v>42.73</v>
       </c>
@@ -3735,13 +3856,17 @@
         <v>5435</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A33" s="8">
         <v>55.52</v>
       </c>
       <c r="B33" s="8">
         <v>19.420000000000002</v>
       </c>
+      <c r="C33" s="13">
+        <f t="shared" si="0"/>
+        <v>74.94</v>
+      </c>
       <c r="D33" s="8">
         <v>25.06</v>
       </c>
@@ -3767,7 +3892,11 @@
         <v>5545</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="C34" s="13">
+        <f t="shared" si="0"/>
+        <v>76.45</v>
+      </c>
       <c r="D34" s="8">
         <v>23.55</v>
       </c>
@@ -3793,13 +3922,17 @@
         <v>5833</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A35" s="8">
         <v>30.7</v>
       </c>
       <c r="B35" s="8">
         <v>43.15</v>
       </c>
+      <c r="C35" s="13">
+        <f t="shared" si="0"/>
+        <v>73.849999999999994</v>
+      </c>
       <c r="D35" s="8">
         <v>26.15</v>
       </c>
@@ -3825,7 +3958,11 @@
         <v>6245</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="C36" s="13">
+        <f t="shared" si="0"/>
+        <v>76</v>
+      </c>
       <c r="D36" s="8">
         <v>24</v>
       </c>
@@ -3859,7 +3996,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I116"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3867,19 +4004,19 @@
       <selection pane="bottomLeft" activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="20.375" customWidth="1"/>
+    <col min="2" max="2" width="20.33203125" customWidth="1"/>
     <col min="3" max="3" width="13" customWidth="1"/>
-    <col min="4" max="4" width="8.375" customWidth="1"/>
-    <col min="5" max="5" width="7.25" customWidth="1"/>
-    <col min="6" max="6" width="4.875" style="7" customWidth="1"/>
-    <col min="7" max="7" width="4.875" customWidth="1"/>
-    <col min="8" max="8" width="14.625" customWidth="1"/>
-    <col min="9" max="9" width="23.25" customWidth="1"/>
+    <col min="4" max="4" width="8.33203125" customWidth="1"/>
+    <col min="5" max="5" width="7.1640625" customWidth="1"/>
+    <col min="6" max="6" width="4.83203125" style="7" customWidth="1"/>
+    <col min="7" max="7" width="4.83203125" customWidth="1"/>
+    <col min="8" max="8" width="14.6640625" customWidth="1"/>
+    <col min="9" max="9" width="23.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>119</v>
       </c>
@@ -3908,7 +4045,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -3923,7 +4060,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -3937,7 +4074,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>126</v>
       </c>
@@ -3951,7 +4088,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>126</v>
       </c>
@@ -3965,7 +4102,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>126</v>
       </c>
@@ -3982,7 +4119,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>126</v>
       </c>
@@ -3999,7 +4136,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>126</v>
       </c>
@@ -4016,7 +4153,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -4033,7 +4170,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>5</v>
       </c>
@@ -4050,7 +4187,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>5</v>
       </c>
@@ -4067,7 +4204,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>5</v>
       </c>
@@ -4084,7 +4221,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>5</v>
       </c>
@@ -4101,7 +4238,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>5</v>
       </c>
@@ -4118,7 +4255,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>5</v>
       </c>
@@ -4135,7 +4272,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>5</v>
       </c>
@@ -4152,7 +4289,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>5</v>
       </c>
@@ -4169,7 +4306,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>5</v>
       </c>
@@ -4186,7 +4323,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>5</v>
       </c>
@@ -4203,7 +4340,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>5</v>
       </c>
@@ -4220,7 +4357,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>5</v>
       </c>
@@ -4237,7 +4374,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>5</v>
       </c>
@@ -4254,7 +4391,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>5</v>
       </c>
@@ -4271,7 +4408,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>5</v>
       </c>
@@ -4288,7 +4425,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>5</v>
       </c>
@@ -4305,7 +4442,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>5</v>
       </c>
@@ -4322,7 +4459,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>5</v>
       </c>
@@ -4339,7 +4476,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>5</v>
       </c>
@@ -4356,7 +4493,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>5</v>
       </c>
@@ -4373,7 +4510,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>5</v>
       </c>
@@ -4391,7 +4528,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>5</v>
       </c>
@@ -4408,7 +4545,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>5</v>
       </c>
@@ -4426,7 +4563,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>5</v>
       </c>
@@ -4443,7 +4580,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>5</v>
       </c>
@@ -4460,7 +4597,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>5</v>
       </c>
@@ -4477,7 +4614,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>5</v>
       </c>
@@ -4494,7 +4631,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>5</v>
       </c>
@@ -4511,7 +4648,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>5</v>
       </c>
@@ -4528,7 +4665,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>5</v>
       </c>
@@ -4545,7 +4682,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>5</v>
       </c>
@@ -4562,7 +4699,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>5</v>
       </c>
@@ -4580,7 +4717,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>5</v>
       </c>
@@ -4597,7 +4734,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>5</v>
       </c>
@@ -4615,7 +4752,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>5</v>
       </c>
@@ -4632,7 +4769,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>5</v>
       </c>
@@ -4650,7 +4787,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>124</v>
       </c>
@@ -4667,7 +4804,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>124</v>
       </c>
@@ -4684,7 +4821,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>125</v>
       </c>
@@ -4698,7 +4835,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>5</v>
       </c>
@@ -4715,7 +4852,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>5</v>
       </c>
@@ -4732,7 +4869,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>5</v>
       </c>
@@ -4749,7 +4886,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>5</v>
       </c>
@@ -4766,7 +4903,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>5</v>
       </c>
@@ -4783,7 +4920,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>5</v>
       </c>
@@ -4800,7 +4937,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>5</v>
       </c>
@@ -4817,7 +4954,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>5</v>
       </c>
@@ -4834,7 +4971,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>5</v>
       </c>
@@ -4851,7 +4988,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>5</v>
       </c>
@@ -4868,7 +5005,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>5</v>
       </c>
@@ -4885,7 +5022,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>5</v>
       </c>
@@ -4902,7 +5039,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>5</v>
       </c>
@@ -4919,7 +5056,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>5</v>
       </c>
@@ -4936,7 +5073,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>5</v>
       </c>
@@ -4953,7 +5090,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>5</v>
       </c>
@@ -4970,7 +5107,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>5</v>
       </c>
@@ -4987,7 +5124,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>5</v>
       </c>
@@ -5004,7 +5141,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>5</v>
       </c>
@@ -5021,7 +5158,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>5</v>
       </c>
@@ -5038,7 +5175,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>5</v>
       </c>
@@ -5055,7 +5192,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>5</v>
       </c>
@@ -5072,7 +5209,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>5</v>
       </c>
@@ -5089,7 +5226,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>5</v>
       </c>
@@ -5106,7 +5243,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>5</v>
       </c>
@@ -5123,7 +5260,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>5</v>
       </c>
@@ -5140,7 +5277,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>5</v>
       </c>
@@ -5157,7 +5294,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>5</v>
       </c>
@@ -5174,7 +5311,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>5</v>
       </c>
@@ -5191,7 +5328,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>5</v>
       </c>
@@ -5208,7 +5345,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>5</v>
       </c>
@@ -5225,7 +5362,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>5</v>
       </c>
@@ -5242,7 +5379,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>5</v>
       </c>
@@ -5259,7 +5396,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>5</v>
       </c>
@@ -5276,7 +5413,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>5</v>
       </c>
@@ -5293,7 +5430,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>5</v>
       </c>
@@ -5310,7 +5447,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>5</v>
       </c>
@@ -5327,7 +5464,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>5</v>
       </c>
@@ -5344,7 +5481,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>5</v>
       </c>
@@ -5361,7 +5498,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>5</v>
       </c>
@@ -5378,7 +5515,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>5</v>
       </c>
@@ -5395,7 +5532,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>5</v>
       </c>
@@ -5412,7 +5549,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>5</v>
       </c>
@@ -5429,7 +5566,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>5</v>
       </c>
@@ -5446,7 +5583,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>5</v>
       </c>
@@ -5463,7 +5600,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>5</v>
       </c>
@@ -5480,7 +5617,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>5</v>
       </c>
@@ -5497,7 +5634,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>5</v>
       </c>
@@ -5514,7 +5651,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>5</v>
       </c>
@@ -5531,7 +5668,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>5</v>
       </c>
@@ -5548,7 +5685,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>5</v>
       </c>
@@ -5565,7 +5702,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>5</v>
       </c>
@@ -5582,7 +5719,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>5</v>
       </c>
@@ -5599,7 +5736,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>5</v>
       </c>
@@ -5616,7 +5753,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>5</v>
       </c>
@@ -5633,7 +5770,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>5</v>
       </c>
@@ -5650,7 +5787,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>5</v>
       </c>
@@ -5667,7 +5804,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>5</v>
       </c>
@@ -5684,7 +5821,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>5</v>
       </c>
@@ -5701,7 +5838,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>5</v>
       </c>
@@ -5719,7 +5856,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>5</v>
       </c>
@@ -5737,7 +5874,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>5</v>
       </c>
@@ -5755,7 +5892,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>5</v>
       </c>
@@ -5773,7 +5910,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>5</v>
       </c>
@@ -5791,7 +5928,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>5</v>
       </c>
@@ -5809,7 +5946,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>5</v>
       </c>
@@ -5830,7 +5967,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>5</v>
       </c>
@@ -5844,7 +5981,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>5</v>
       </c>
@@ -5865,22 +6002,22 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:DE89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
+    <sheetView topLeftCell="A18" workbookViewId="0">
       <selection activeCell="AC14" sqref="AC14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="11.125" customWidth="1"/>
+    <col min="2" max="2" width="11.1640625" customWidth="1"/>
     <col min="22" max="22" width="9" style="9"/>
     <col min="50" max="51" width="9" style="9"/>
     <col min="87" max="90" width="9" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:109" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:109" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>192</v>
       </c>
@@ -6209,7 +6346,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="2" spans="1:109" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:109" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>109</v>
       </c>
@@ -6352,7 +6489,7 @@
         <v>617</v>
       </c>
     </row>
-    <row r="3" spans="1:109" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:109" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>110</v>
       </c>
@@ -6495,7 +6632,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="4" spans="1:109" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:109" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>111</v>
       </c>
@@ -6638,7 +6775,7 @@
         <v>1358</v>
       </c>
     </row>
-    <row r="5" spans="1:109" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:109" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>805</v>
       </c>
@@ -6733,7 +6870,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="6" spans="1:109" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:109" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>806</v>
       </c>
@@ -6828,7 +6965,7 @@
         <v>821</v>
       </c>
     </row>
-    <row r="7" spans="1:109" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:109" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1024</v>
       </c>
@@ -6923,7 +7060,7 @@
         <v>10.7</v>
       </c>
     </row>
-    <row r="8" spans="1:109" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:109" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1025</v>
       </c>
@@ -7015,7 +7152,7 @@
         <v>-38</v>
       </c>
     </row>
-    <row r="9" spans="1:109" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:109" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>1086</v>
       </c>
@@ -7194,7 +7331,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="10" spans="1:109" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:109" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>1499</v>
       </c>
@@ -7280,7 +7417,7 @@
         <v>1677</v>
       </c>
     </row>
-    <row r="11" spans="1:109" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:109" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>1513</v>
       </c>
@@ -7387,7 +7524,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="12" spans="1:109" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:109" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>1514</v>
       </c>
@@ -7491,7 +7628,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="13" spans="1:109" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:109" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>1515</v>
       </c>
@@ -7595,7 +7732,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="14" spans="1:109" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:109" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>1516</v>
       </c>
@@ -7702,7 +7839,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="15" spans="1:109" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:109" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>1571</v>
       </c>
@@ -7806,7 +7943,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="16" spans="1:109" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:109" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>1572</v>
       </c>
@@ -7910,7 +8047,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="17" spans="1:109" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:109" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>1573</v>
       </c>
@@ -8014,7 +8151,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="18" spans="1:109" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:109" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>1574</v>
       </c>
@@ -8118,7 +8255,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="19" spans="1:109" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:109" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>1637</v>
       </c>
@@ -8210,7 +8347,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="20" spans="1:109" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:109" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>1638</v>
       </c>
@@ -8305,7 +8442,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:109" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:109" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>1794</v>
       </c>
@@ -8427,7 +8564,7 @@
         <v>189000</v>
       </c>
     </row>
-    <row r="22" spans="1:109" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:109" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>1880</v>
       </c>
@@ -8507,7 +8644,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:109" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:109" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>2088</v>
       </c>
@@ -8596,7 +8733,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:109" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:109" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>2089</v>
       </c>
@@ -8676,7 +8813,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:109" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:109" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>2090</v>
       </c>
@@ -8756,7 +8893,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="26" spans="1:109" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:109" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>2107</v>
       </c>
@@ -8890,7 +9027,7 @@
         <v>5420</v>
       </c>
     </row>
-    <row r="27" spans="1:109" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:109" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>2108</v>
       </c>
@@ -9006,7 +9143,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="28" spans="1:109" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:109" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>2109</v>
       </c>
@@ -9131,7 +9268,7 @@
         <v>8120</v>
       </c>
     </row>
-    <row r="29" spans="1:109" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:109" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>2112</v>
       </c>
@@ -9265,7 +9402,7 @@
         <v>5990</v>
       </c>
     </row>
-    <row r="30" spans="1:109" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:109" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>2113</v>
       </c>
@@ -9399,7 +9536,7 @@
         <v>5890</v>
       </c>
     </row>
-    <row r="31" spans="1:109" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:109" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>2123</v>
       </c>
@@ -9521,7 +9658,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="32" spans="1:109" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:109" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>2124</v>
       </c>
@@ -9649,7 +9786,7 @@
         <v>3.6</v>
       </c>
     </row>
-    <row r="33" spans="1:109" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:109" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>2126</v>
       </c>
@@ -9777,7 +9914,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="34" spans="1:109" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:109" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>2394</v>
       </c>
@@ -9881,7 +10018,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="35" spans="1:109" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:109" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>2403</v>
       </c>
@@ -9976,7 +10113,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="36" spans="1:109" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:109" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>2404</v>
       </c>
@@ -10071,7 +10208,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="37" spans="1:109" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:109" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>3087</v>
       </c>
@@ -10208,7 +10345,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="38" spans="1:109" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:109" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>3347</v>
       </c>
@@ -10294,7 +10431,7 @@
         <v>1160</v>
       </c>
     </row>
-    <row r="39" spans="1:109" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:109" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>3404</v>
       </c>
@@ -10386,7 +10523,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="40" spans="1:109" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:109" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>3405</v>
       </c>
@@ -10478,7 +10615,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="41" spans="1:109" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:109" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>3406</v>
       </c>
@@ -10570,7 +10707,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="42" spans="1:109" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:109" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>3892</v>
       </c>
@@ -10662,7 +10799,7 @@
         <v>2.2000000000000002</v>
       </c>
     </row>
-    <row r="43" spans="1:109" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:109" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>3893</v>
       </c>
@@ -10754,7 +10891,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="44" spans="1:109" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:109" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>3894</v>
       </c>
@@ -10846,7 +10983,7 @@
         <v>6.7</v>
       </c>
     </row>
-    <row r="45" spans="1:109" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:109" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>3895</v>
       </c>
@@ -10938,7 +11075,7 @@
         <v>8.8000000000000007</v>
       </c>
     </row>
-    <row r="46" spans="1:109" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:109" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>4121</v>
       </c>
@@ -11039,7 +11176,7 @@
         <v>123.3</v>
       </c>
     </row>
-    <row r="47" spans="1:109" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:109" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>4122</v>
       </c>
@@ -11140,7 +11277,7 @@
         <v>88.5</v>
       </c>
     </row>
-    <row r="48" spans="1:109" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:109" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>4123</v>
       </c>
@@ -11238,7 +11375,7 @@
         <v>147.4</v>
       </c>
     </row>
-    <row r="49" spans="1:108" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:108" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>4124</v>
       </c>
@@ -11336,7 +11473,7 @@
         <v>147.80000000000001</v>
       </c>
     </row>
-    <row r="50" spans="1:108" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:108" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>4164</v>
       </c>
@@ -11458,7 +11595,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="51" spans="1:108" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:108" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>4165</v>
       </c>
@@ -11562,7 +11699,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="52" spans="1:108" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:108" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>4166</v>
       </c>
@@ -11669,7 +11806,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="53" spans="1:108" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:108" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>4167</v>
       </c>
@@ -11788,7 +11925,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="54" spans="1:108" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:108" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>4340</v>
       </c>
@@ -11898,7 +12035,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="55" spans="1:108" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:108" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>5671</v>
       </c>
@@ -11993,7 +12130,7 @@
         <v>1540</v>
       </c>
     </row>
-    <row r="56" spans="1:108" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:108" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>5756</v>
       </c>
@@ -12106,7 +12243,7 @@
         <v>-287</v>
       </c>
     </row>
-    <row r="57" spans="1:108" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:108" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>5757</v>
       </c>
@@ -12219,7 +12356,7 @@
         <v>-303</v>
       </c>
     </row>
-    <row r="58" spans="1:108" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:108" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>5758</v>
       </c>
@@ -12332,7 +12469,7 @@
         <v>-339</v>
       </c>
     </row>
-    <row r="59" spans="1:108" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:108" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>5759</v>
       </c>
@@ -12445,7 +12582,7 @@
         <v>-297</v>
       </c>
     </row>
-    <row r="60" spans="1:108" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:108" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>5760</v>
       </c>
@@ -12558,7 +12695,7 @@
         <v>-403</v>
       </c>
     </row>
-    <row r="61" spans="1:108" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:108" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>5761</v>
       </c>
@@ -12680,7 +12817,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="62" spans="1:108" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:108" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>5762</v>
       </c>
@@ -12802,7 +12939,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="63" spans="1:108" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:108" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>5763</v>
       </c>
@@ -12924,7 +13061,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="64" spans="1:108" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:108" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>5764</v>
       </c>
@@ -13046,7 +13183,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="65" spans="1:105" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:105" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>5765</v>
       </c>
@@ -13168,7 +13305,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="66" spans="1:105" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:105" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>5766</v>
       </c>
@@ -13287,7 +13424,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="67" spans="1:105" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:105" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>5767</v>
       </c>
@@ -13387,7 +13524,7 @@
       <c r="AP67">
         <v>186</v>
       </c>
-      <c r="CI67" s="19">
+      <c r="CI67" s="12">
         <v>1000</v>
       </c>
       <c r="CJ67" s="9">
@@ -13406,7 +13543,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="68" spans="1:105" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:105" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>5768</v>
       </c>
@@ -13525,7 +13662,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="69" spans="1:105" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:105" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>5769</v>
       </c>
@@ -13644,7 +13781,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="70" spans="1:105" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:105" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>5770</v>
       </c>
@@ -13763,7 +13900,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="71" spans="1:105" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:105" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>6334</v>
       </c>
@@ -13879,7 +14016,7 @@
         <v>205.25</v>
       </c>
     </row>
-    <row r="72" spans="1:105" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:105" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>6335</v>
       </c>
@@ -13995,7 +14132,7 @@
         <v>205.25</v>
       </c>
     </row>
-    <row r="73" spans="1:105" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:105" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>6336</v>
       </c>
@@ -14111,7 +14248,7 @@
         <v>205.25</v>
       </c>
     </row>
-    <row r="74" spans="1:105" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:105" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>6337</v>
       </c>
@@ -14230,7 +14367,7 @@
         <v>178.5</v>
       </c>
     </row>
-    <row r="75" spans="1:105" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:105" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>6338</v>
       </c>
@@ -14349,7 +14486,7 @@
         <v>178.5</v>
       </c>
     </row>
-    <row r="76" spans="1:105" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:105" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>6339</v>
       </c>
@@ -14468,7 +14605,7 @@
         <v>178.5</v>
       </c>
     </row>
-    <row r="77" spans="1:105" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:105" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>6340</v>
       </c>
@@ -14587,7 +14724,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="78" spans="1:105" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:105" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>6341</v>
       </c>
@@ -14706,7 +14843,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="79" spans="1:105" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:105" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>6342</v>
       </c>
@@ -14825,7 +14962,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="80" spans="1:105" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:105" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>6343</v>
       </c>
@@ -14944,7 +15081,7 @@
         <v>223.75</v>
       </c>
     </row>
-    <row r="81" spans="1:108" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:108" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>6344</v>
       </c>
@@ -15063,7 +15200,7 @@
         <v>223.75</v>
       </c>
     </row>
-    <row r="82" spans="1:108" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:108" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>6345</v>
       </c>
@@ -15182,7 +15319,7 @@
         <v>223.75</v>
       </c>
     </row>
-    <row r="83" spans="1:108" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:108" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>6346</v>
       </c>
@@ -15304,7 +15441,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="84" spans="1:108" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:108" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>6347</v>
       </c>
@@ -15426,7 +15563,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="85" spans="1:108" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:108" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>6348</v>
       </c>
@@ -15548,7 +15685,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="86" spans="1:108" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:108" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>6349</v>
       </c>
@@ -15670,7 +15807,7 @@
         <v>473.5</v>
       </c>
     </row>
-    <row r="87" spans="1:108" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:108" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>6350</v>
       </c>
@@ -15792,7 +15929,7 @@
         <v>473.5</v>
       </c>
     </row>
-    <row r="88" spans="1:108" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:108" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>6351</v>
       </c>
@@ -15914,7 +16051,7 @@
         <v>473.5</v>
       </c>
     </row>
-    <row r="89" spans="1:108" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:108" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>6516</v>
       </c>
@@ -16079,231 +16216,231 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:DE89"/>
+  <autoFilter ref="A1:DE89" xr:uid="{00000000-0009-0000-0000-000002000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B2:E23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="5" max="5" width="94.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B2" s="1"/>
       <c r="C2" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="D2" s="17" t="s">
+      <c r="D2" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="E2" s="18"/>
-    </row>
-    <row r="3" spans="2:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="12" t="s">
+      <c r="E2" s="20"/>
+    </row>
+    <row r="3" spans="2:5" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B3" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="14"/>
-    </row>
-    <row r="4" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="16"/>
+    </row>
+    <row r="4" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="3"/>
       <c r="C4" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="D4" s="15" t="s">
+      <c r="D4" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="E4" s="16"/>
-    </row>
-    <row r="5" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E4" s="18"/>
+    </row>
+    <row r="5" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="3"/>
       <c r="C5" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="D5" s="15" t="s">
+      <c r="D5" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="E5" s="16"/>
-    </row>
-    <row r="6" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E5" s="18"/>
+    </row>
+    <row r="6" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="3"/>
       <c r="C6" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="D6" s="15" t="s">
+      <c r="D6" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="E6" s="16"/>
-    </row>
-    <row r="7" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E6" s="18"/>
+    </row>
+    <row r="7" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="3"/>
       <c r="C7" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="D7" s="15" t="s">
+      <c r="D7" s="17" t="s">
         <v>70</v>
       </c>
-      <c r="E7" s="16"/>
-    </row>
-    <row r="8" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E7" s="18"/>
+    </row>
+    <row r="8" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="3"/>
       <c r="C8" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="D8" s="15" t="s">
+      <c r="D8" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="E8" s="16"/>
-    </row>
-    <row r="9" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E8" s="18"/>
+    </row>
+    <row r="9" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="3"/>
       <c r="C9" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="D9" s="15" t="s">
+      <c r="D9" s="17" t="s">
         <v>74</v>
       </c>
-      <c r="E9" s="16"/>
-    </row>
-    <row r="10" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E9" s="18"/>
+    </row>
+    <row r="10" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="3"/>
       <c r="C10" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="D10" s="15" t="s">
+      <c r="D10" s="17" t="s">
         <v>76</v>
       </c>
-      <c r="E10" s="16"/>
-    </row>
-    <row r="11" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E10" s="18"/>
+    </row>
+    <row r="11" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="3"/>
       <c r="C11" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="D11" s="15" t="s">
+      <c r="D11" s="17" t="s">
         <v>78</v>
       </c>
-      <c r="E11" s="16"/>
-    </row>
-    <row r="12" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E11" s="18"/>
+    </row>
+    <row r="12" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="3"/>
       <c r="C12" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="D12" s="15" t="s">
+      <c r="D12" s="17" t="s">
         <v>80</v>
       </c>
-      <c r="E12" s="16"/>
-    </row>
-    <row r="13" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E12" s="18"/>
+    </row>
+    <row r="13" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="3"/>
       <c r="C13" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="D13" s="15" t="s">
+      <c r="D13" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="E13" s="16"/>
-    </row>
-    <row r="14" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E13" s="18"/>
+    </row>
+    <row r="14" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="3"/>
       <c r="C14" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="D14" s="15" t="s">
+      <c r="D14" s="17" t="s">
         <v>84</v>
       </c>
-      <c r="E14" s="16"/>
-    </row>
-    <row r="15" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E14" s="18"/>
+    </row>
+    <row r="15" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="3"/>
       <c r="C15" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="D15" s="15" t="s">
+      <c r="D15" s="17" t="s">
         <v>86</v>
       </c>
-      <c r="E15" s="16"/>
-    </row>
-    <row r="16" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E15" s="18"/>
+    </row>
+    <row r="16" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="3"/>
       <c r="C16" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="D16" s="15" t="s">
+      <c r="D16" s="17" t="s">
         <v>88</v>
       </c>
-      <c r="E16" s="16"/>
-    </row>
-    <row r="17" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E16" s="18"/>
+    </row>
+    <row r="17" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="3"/>
       <c r="C17" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="D17" s="15" t="s">
+      <c r="D17" s="17" t="s">
         <v>90</v>
       </c>
-      <c r="E17" s="16"/>
-    </row>
-    <row r="18" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E17" s="18"/>
+    </row>
+    <row r="18" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="3"/>
       <c r="C18" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="D18" s="15" t="s">
+      <c r="D18" s="17" t="s">
         <v>92</v>
       </c>
-      <c r="E18" s="16"/>
-    </row>
-    <row r="19" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E18" s="18"/>
+    </row>
+    <row r="19" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="3"/>
       <c r="C19" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="D19" s="15" t="s">
+      <c r="D19" s="17" t="s">
         <v>94</v>
       </c>
-      <c r="E19" s="16"/>
-    </row>
-    <row r="20" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="12" t="s">
+      <c r="E19" s="18"/>
+    </row>
+    <row r="20" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B20" s="14" t="s">
         <v>95</v>
       </c>
-      <c r="C20" s="13"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="14"/>
-    </row>
-    <row r="21" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C20" s="15"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="16"/>
+    </row>
+    <row r="21" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="3"/>
       <c r="C21" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="D21" s="15" t="s">
+      <c r="D21" s="17" t="s">
         <v>97</v>
       </c>
-      <c r="E21" s="16"/>
-    </row>
-    <row r="22" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E21" s="18"/>
+    </row>
+    <row r="22" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B22" s="3"/>
       <c r="C22" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="D22" s="15" t="s">
+      <c r="D22" s="17" t="s">
         <v>99</v>
       </c>
-      <c r="E22" s="16"/>
-    </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E22" s="18"/>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B23" s="6"/>
       <c r="C23" s="6"/>
       <c r="D23" s="6"/>

</xml_diff>